<commit_message>
so much to push
including starting revision for flobuds
</commit_message>
<xml_diff>
--- a/investment/Data/zarchieve/cherry_data.xlsx
+++ b/investment/Data/zarchieve/cherry_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/proterant/investment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/proterant/investment/Data/zarchieve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2399CEA7-9570-FC4B-9AA9-69A7C6BAD618}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EF2833-1377-7D4E-91A5-5B0E9A06C902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="5940" windowWidth="26440" windowHeight="20340" xr2:uid="{1E6EFEBF-EF8B-5847-A336-77C74E2BDC8D}"/>
+    <workbookView xWindow="26200" yWindow="6680" windowWidth="26440" windowHeight="16680" xr2:uid="{1E6EFEBF-EF8B-5847-A336-77C74E2BDC8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7197E432-6299-4544-9B35-C550FFF79A3F}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,7 +753,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>

</xml_diff>